<commit_message>
finished hardware side (test ongoing)
</commit_message>
<xml_diff>
--- a/Instructions_Encoding.xlsx
+++ b/Instructions_Encoding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Files\Personal_Projects\MIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A6FD22-04BB-4A93-A085-5CBE0C8263E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A210AC-1427-437E-8171-0464AE23CB35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -722,8 +722,8 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
first test and debug
</commit_message>
<xml_diff>
--- a/Instructions_Encoding.xlsx
+++ b/Instructions_Encoding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Files\Personal_Projects\MIPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A210AC-1427-437E-8171-0464AE23CB35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AD113E9-A38B-4624-9B82-2E6CC999733F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="77">
   <si>
     <t>Instruction</t>
   </si>
@@ -253,6 +254,9 @@
   </si>
   <si>
     <t>destination = $t</t>
+  </si>
+  <si>
+    <t>0000000000000001 0001100000100000</t>
   </si>
 </sst>
 </file>
@@ -423,6 +427,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -438,7 +443,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,7 +727,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,12 +756,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
       <c r="G2" t="s">
         <v>61</v>
       </c>
@@ -769,7 +773,7 @@
       <c r="B3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="4">
@@ -786,7 +790,7 @@
       <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4">
         <v>100001</v>
       </c>
@@ -801,7 +805,7 @@
       <c r="B5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="4">
         <v>100100</v>
       </c>
@@ -819,7 +823,7 @@
       <c r="B6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="4">
         <v>100111</v>
       </c>
@@ -837,7 +841,7 @@
       <c r="B7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="4">
         <v>100101</v>
       </c>
@@ -852,7 +856,7 @@
       <c r="B8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="10"/>
       <c r="D8" s="4">
         <v>0</v>
       </c>
@@ -864,7 +868,7 @@
       <c r="B9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="4">
         <v>100</v>
       </c>
@@ -876,7 +880,7 @@
       <c r="B10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="4">
         <v>11</v>
       </c>
@@ -888,9 +892,12 @@
       <c r="B11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="4">
         <v>111</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -900,7 +907,7 @@
       <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="4">
         <v>10</v>
       </c>
@@ -912,7 +919,7 @@
       <c r="B13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="4">
         <v>110</v>
       </c>
@@ -924,7 +931,7 @@
       <c r="B14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="4">
         <v>100010</v>
       </c>
@@ -936,7 +943,7 @@
       <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="4">
         <v>100011</v>
       </c>
@@ -948,7 +955,7 @@
       <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="4">
         <v>100110</v>
       </c>
@@ -960,7 +967,7 @@
       <c r="B17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="4">
         <v>101010</v>
       </c>
@@ -972,7 +979,7 @@
       <c r="B18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="4">
         <v>101001</v>
       </c>
@@ -984,12 +991,12 @@
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
       <c r="G20" t="s">
         <v>62</v>
       </c>
@@ -1112,52 +1119,52 @@
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="9">
         <v>100000</v>
       </c>
-      <c r="D29" s="14"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="9">
         <v>100100</v>
       </c>
-      <c r="D30" s="14"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="9">
         <v>100001</v>
       </c>
-      <c r="D31" s="14"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="9">
         <v>100101</v>
       </c>
-      <c r="D32" s="14"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
@@ -1172,28 +1179,28 @@
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="9">
         <v>101000</v>
       </c>
-      <c r="D34" s="14"/>
+      <c r="D34" s="9"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="9">
         <v>101001</v>
       </c>
-      <c r="D35" s="14"/>
+      <c r="D35" s="9"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">

</xml_diff>